<commit_message>
Completed migrating to Oracle
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/API Interface/Backend.xlsx
+++ b/Specifications (仕様書)/API Interface/Backend.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet name="Tổng quan" sheetId="1" r:id="rId1"/>
     <sheet name="Quản Lý Cư Trú" sheetId="2" r:id="rId2"/>
-    <sheet name="Quản Lý Dân" sheetId="3" r:id="rId3"/>
+    <sheet name="Quản Lý Dân DO" sheetId="5" r:id="rId3"/>
+    <sheet name="Quản Lý Dân" sheetId="3" r:id="rId4"/>
+    <sheet name="Quản Lý Cư Trú DO" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>Tác giả:</t>
   </si>
@@ -240,6 +242,9 @@
   </si>
   <si>
     <t>getCuTrusByPersonalAddress(diaChiDan)</t>
+  </si>
+  <si>
+    <t>Q</t>
   </si>
 </sst>
 </file>
@@ -660,7 +665,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -936,10 +941,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1091,4 +1114,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified specs, Implemented some backend logics
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/API Interface/Backend.xlsx
+++ b/Specifications (仕様書)/API Interface/Backend.xlsx
@@ -4,15 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quan" sheetId="1" r:id="rId1"/>
     <sheet name="Quản Lý Cư Trú" sheetId="2" r:id="rId2"/>
-    <sheet name="Quản Lý Dân DO" sheetId="5" r:id="rId3"/>
-    <sheet name="Quản Lý Dân" sheetId="3" r:id="rId4"/>
-    <sheet name="Quản Lý Cư Trú DO" sheetId="4" r:id="rId5"/>
+    <sheet name="Quản Lý Dân" sheetId="3" r:id="rId3"/>
+    <sheet name="Data Object" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="CuTruDO">'Data Object'!$B$5</definedName>
+    <definedName name="NguoiDungDO">'Data Object'!$B$25</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
   <si>
     <t>Tác giả:</t>
   </si>
@@ -73,9 +76,6 @@
     <t>Lấy danh sách cư trú</t>
   </si>
   <si>
-    <t>Lấy danh sách cư trú theo id</t>
-  </si>
-  <si>
     <t>Tìm kiếm cư trú theo loại cư trú</t>
   </si>
   <si>
@@ -244,14 +244,206 @@
     <t>getCuTrusByPersonalAddress(diaChiDan)</t>
   </si>
   <si>
-    <t>Q</t>
+    <t>カラム名</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ngayTao</t>
+  </si>
+  <si>
+    <t>ngayDangKy</t>
+  </si>
+  <si>
+    <t>ngayHetHan</t>
+  </si>
+  <si>
+    <t>dienThoai</t>
+  </si>
+  <si>
+    <t>soNha</t>
+  </si>
+  <si>
+    <t>duong</t>
+  </si>
+  <si>
+    <t>phuong</t>
+  </si>
+  <si>
+    <t>quan</t>
+  </si>
+  <si>
+    <t>thanhPho</t>
+  </si>
+  <si>
+    <t>daDuyet</t>
+  </si>
+  <si>
+    <t>loaiCuTruId</t>
+  </si>
+  <si>
+    <t>canBoId</t>
+  </si>
+  <si>
+    <t>説明</t>
+  </si>
+  <si>
+    <t>データ種別</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>congDans</t>
+  </si>
+  <si>
+    <t>CuTru</t>
+  </si>
+  <si>
+    <t>Dữ liệu trả về</t>
+  </si>
+  <si>
+    <t>[CuTru]</t>
+  </si>
+  <si>
+    <t>Lấy cư trú theo id</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>Mã số cư trú</t>
+  </si>
+  <si>
+    <t>Ngày tạo</t>
+  </si>
+  <si>
+    <t>Ngày đăng ký</t>
+  </si>
+  <si>
+    <t>Ngày hết hạn</t>
+  </si>
+  <si>
+    <t>Điện thoại</t>
+  </si>
+  <si>
+    <t>Số nhà</t>
+  </si>
+  <si>
+    <t>Đường</t>
+  </si>
+  <si>
+    <t>Phường</t>
+  </si>
+  <si>
+    <t>Quận</t>
+  </si>
+  <si>
+    <t>Thành Phố</t>
+  </si>
+  <si>
+    <t>Trạng thái duyệt</t>
+  </si>
+  <si>
+    <t>Mã loại cư trú</t>
+  </si>
+  <si>
+    <t>Mã cán bộ duyệt</t>
+  </si>
+  <si>
+    <t>Danh sách công dân</t>
+  </si>
+  <si>
+    <t>対象名</t>
+  </si>
+  <si>
+    <t>Lưu thông tin cư trú</t>
+  </si>
+  <si>
+    <t>[NguoiDung]</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>NguoiDung</t>
+  </si>
+  <si>
+    <t>Lưu thông tin người dùng</t>
+  </si>
+  <si>
+    <t>hoTen</t>
+  </si>
+  <si>
+    <t>gioiTinh</t>
+  </si>
+  <si>
+    <t>sinhNhat</t>
+  </si>
+  <si>
+    <t>noiSinh</t>
+  </si>
+  <si>
+    <t>queQuan</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>identityId</t>
+  </si>
+  <si>
+    <t>quocTich</t>
+  </si>
+  <si>
+    <t>chucVuId</t>
+  </si>
+  <si>
+    <t>Mã số công dân</t>
+  </si>
+  <si>
+    <t>Họ tên</t>
+  </si>
+  <si>
+    <t>Sinh nhật</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Nơi sinh</t>
+  </si>
+  <si>
+    <t>Quê quán</t>
+  </si>
+  <si>
+    <t>Quốc tịch</t>
+  </si>
+  <si>
+    <t>Ảnh đại diện</t>
+  </si>
+  <si>
+    <t>Mã xác thực</t>
+  </si>
+  <si>
+    <t>Mã chức vụ</t>
+  </si>
+  <si>
+    <t>/{id}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,8 +471,23 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,8 +500,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -302,11 +521,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -315,8 +615,30 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -597,14 +919,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="22.8" x14ac:dyDescent="0.4">
@@ -651,7 +973,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="5">
-        <v>43357</v>
+        <v>43365</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -662,10 +984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -675,10 +997,11 @@
     <col min="3" max="3" width="16.88671875" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="6" max="6" width="16.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -694,8 +1017,11 @@
       <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -711,13 +1037,16 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -726,214 +1055,267 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>39</v>
+      <c r="F15" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F3" location="CuTruDO" display="CuTru"/>
+    <hyperlink ref="F4" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F5" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F6" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F8" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F10" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F12" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F7" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F9" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F11" location="CuTruDO" display="[CuTru]"/>
+    <hyperlink ref="F13" location="CuTruDO" display="CuTru"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -941,28 +1323,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -997,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -1006,7 +1370,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1014,16 +1378,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1031,16 +1395,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1048,16 +1412,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1065,16 +1429,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1082,16 +1446,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1099,16 +1463,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1116,16 +1480,414 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A5:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="19"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="22"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>